<commit_message>
Complete the function of admin insert the school grade teacher information and register user.
</commit_message>
<xml_diff>
--- a/src/main/webapp/static/excel/class.xlsx
+++ b/src/main/webapp/static/excel/class.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\images-gather\src\main\webapp\static\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\images-gather\src\main\webapp\static\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E6B825-9A68-48FA-A012-E859ECC76E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24978327-FAE8-4219-87AD-E7B95B6D14E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -404,7 +404,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,12 +446,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rXBJhFwP1CMewuVJSU2q6rx5tOuvWyiaQ5k6VVzA8tycOkORjCb2MCo7Ik6fPh1o2/+lneh/i2qnfprF4bShLA==" saltValue="qOcwunyVrmQPUaNA263qsQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{6B41C828-E3A1-473D-A090-114F83930DC5}">
       <formula1>"男,女"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{C59CAB79-AB32-4DAF-BDD7-979DB4052A3D}">
-      <formula1>"班长"</formula1>
+      <formula1>"班长,班主任"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>